<commit_message>
Cleaned up some stuff added Base Design Document (Basis Ontwerp) Also changed the style and look of the dashboard sketch
</commit_message>
<xml_diff>
--- a/Documentatie/Cheery Gantt Planner.xlsx
+++ b/Documentatie/Cheery Gantt Planner.xlsx
@@ -190,9 +190,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="d/m;@"/>
+    <numFmt numFmtId="164" formatCode="d/m;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -298,6 +298,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFC00000"/>
+      <name val="Corbel"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
       <name val="Corbel"/>
       <family val="2"/>
       <scheme val="major"/>
@@ -429,7 +436,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -511,9 +518,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -523,7 +527,13 @@
     <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -537,248 +547,7 @@
     <cellStyle name="Period Highlight Control" xfId="7"/>
     <cellStyle name="Project Headers" xfId="4"/>
   </cellStyles>
-  <dxfs count="39">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="7"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="7"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="7"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color theme="7"/>
-        </top>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
@@ -913,125 +682,32 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border>
         <top style="thin">
           <color theme="7"/>
         </top>
         <vertical/>
         <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -1059,8 +735,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="38"/>
-      <tableStyleElement type="headerRow" dxfId="37"/>
+      <tableStyleElement type="wholeTable" dxfId="13"/>
+      <tableStyleElement type="headerRow" dxfId="12"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1084,7 +760,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="4"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Spin" dx="16" fmlaLink="period_selected" max="60" min="1" page="10" val="11"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1369,10 +1045,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:BZ41"/>
+  <dimension ref="B2:DE41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.75" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -1405,25 +1081,26 @@
     <col min="76" max="76" width="5.125" bestFit="1" customWidth="1"/>
     <col min="77" max="77" width="5.25" bestFit="1" customWidth="1"/>
     <col min="78" max="78" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="79" max="109" width="4.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:78" ht="15" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
+    <row r="2" spans="2:109" ht="15" x14ac:dyDescent="0.25">
+      <c r="B2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
     </row>
-    <row r="3" spans="2:78" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
+    <row r="3" spans="2:109" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
       <c r="I3" s="8" t="s">
         <v>13</v>
       </c>
@@ -1432,7 +1109,7 @@
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="9">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="O3" s="8"/>
       <c r="Q3" s="10"/>
@@ -1460,20 +1137,20 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:78" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
+    <row r="4" spans="2:109" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
       <c r="AT4" s="1"/>
       <c r="AU4" s="1"/>
       <c r="AV4" s="1"/>
       <c r="AW4" s="1"/>
       <c r="AX4" s="1"/>
     </row>
-    <row r="5" spans="2:78" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:109" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1481,10 +1158,10 @@
         <f>DATE(2015,10,7)</f>
         <v>42284</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="29">
         <f>DATE(2015,12,15)</f>
         <v>42353</v>
       </c>
@@ -1492,325 +1169,325 @@
       <c r="AU5" s="1"/>
       <c r="AV5" s="1"/>
     </row>
-    <row r="6" spans="2:78" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:109" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="26">
         <f ca="1">NOW()</f>
-        <v>42302.760482291669</v>
+        <v>42309.702942129632</v>
       </c>
       <c r="AT6" s="1"/>
       <c r="AU6" s="1"/>
       <c r="AV6" s="1"/>
     </row>
-    <row r="7" spans="2:78" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:109" x14ac:dyDescent="0.3">
       <c r="AT7" s="1"/>
       <c r="AU7" s="1"/>
       <c r="AV7" s="1"/>
     </row>
-    <row r="8" spans="2:78" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:109" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="27">
         <f ca="1">E5-C6</f>
-        <v>50.239517708330823</v>
+        <v>43.297057870368008</v>
       </c>
       <c r="AT8" s="1"/>
       <c r="AU8" s="1"/>
       <c r="AV8" s="1"/>
     </row>
-    <row r="9" spans="2:78" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:109" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="27">
         <f ca="1">C6-C5</f>
-        <v>18.760482291669177</v>
-      </c>
-      <c r="I9" s="31">
+        <v>25.702942129631992</v>
+      </c>
+      <c r="I9" s="30">
         <f>C5</f>
         <v>42284</v>
       </c>
-      <c r="J9" s="31">
+      <c r="J9" s="30">
         <f>I9+1</f>
         <v>42285</v>
       </c>
-      <c r="K9" s="31">
+      <c r="K9" s="30">
         <f t="shared" ref="K9:BV9" si="0">J9+1</f>
         <v>42286</v>
       </c>
-      <c r="L9" s="31">
+      <c r="L9" s="30">
         <f t="shared" si="0"/>
         <v>42287</v>
       </c>
-      <c r="M9" s="31">
+      <c r="M9" s="30">
         <f t="shared" si="0"/>
         <v>42288</v>
       </c>
-      <c r="N9" s="31">
+      <c r="N9" s="30">
         <f t="shared" si="0"/>
         <v>42289</v>
       </c>
-      <c r="O9" s="31">
+      <c r="O9" s="30">
         <f t="shared" si="0"/>
         <v>42290</v>
       </c>
-      <c r="P9" s="31">
+      <c r="P9" s="30">
         <f t="shared" si="0"/>
         <v>42291</v>
       </c>
-      <c r="Q9" s="31">
+      <c r="Q9" s="30">
         <f t="shared" si="0"/>
         <v>42292</v>
       </c>
-      <c r="R9" s="31">
+      <c r="R9" s="30">
         <f t="shared" si="0"/>
         <v>42293</v>
       </c>
-      <c r="S9" s="31">
+      <c r="S9" s="30">
         <f t="shared" si="0"/>
         <v>42294</v>
       </c>
-      <c r="T9" s="31">
+      <c r="T9" s="30">
         <f t="shared" si="0"/>
         <v>42295</v>
       </c>
-      <c r="U9" s="31">
+      <c r="U9" s="30">
         <f t="shared" si="0"/>
         <v>42296</v>
       </c>
-      <c r="V9" s="31">
+      <c r="V9" s="30">
         <f t="shared" si="0"/>
         <v>42297</v>
       </c>
-      <c r="W9" s="31">
+      <c r="W9" s="30">
         <f t="shared" si="0"/>
         <v>42298</v>
       </c>
-      <c r="X9" s="31">
+      <c r="X9" s="30">
         <f t="shared" si="0"/>
         <v>42299</v>
       </c>
-      <c r="Y9" s="31">
+      <c r="Y9" s="30">
         <f t="shared" si="0"/>
         <v>42300</v>
       </c>
-      <c r="Z9" s="31">
+      <c r="Z9" s="30">
         <f t="shared" si="0"/>
         <v>42301</v>
       </c>
-      <c r="AA9" s="31">
+      <c r="AA9" s="30">
         <f t="shared" si="0"/>
         <v>42302</v>
       </c>
-      <c r="AB9" s="31">
+      <c r="AB9" s="30">
         <f t="shared" si="0"/>
         <v>42303</v>
       </c>
-      <c r="AC9" s="31">
+      <c r="AC9" s="30">
         <f t="shared" si="0"/>
         <v>42304</v>
       </c>
-      <c r="AD9" s="31">
+      <c r="AD9" s="30">
         <f t="shared" si="0"/>
         <v>42305</v>
       </c>
-      <c r="AE9" s="31">
+      <c r="AE9" s="30">
         <f t="shared" si="0"/>
         <v>42306</v>
       </c>
-      <c r="AF9" s="31">
+      <c r="AF9" s="30">
         <f t="shared" si="0"/>
         <v>42307</v>
       </c>
-      <c r="AG9" s="31">
+      <c r="AG9" s="30">
         <f t="shared" si="0"/>
         <v>42308</v>
       </c>
-      <c r="AH9" s="31">
+      <c r="AH9" s="30">
         <f t="shared" si="0"/>
         <v>42309</v>
       </c>
-      <c r="AI9" s="31">
+      <c r="AI9" s="30">
         <f t="shared" si="0"/>
         <v>42310</v>
       </c>
-      <c r="AJ9" s="31">
+      <c r="AJ9" s="30">
         <f t="shared" si="0"/>
         <v>42311</v>
       </c>
-      <c r="AK9" s="31">
+      <c r="AK9" s="30">
         <f t="shared" si="0"/>
         <v>42312</v>
       </c>
-      <c r="AL9" s="31">
+      <c r="AL9" s="30">
         <f t="shared" si="0"/>
         <v>42313</v>
       </c>
-      <c r="AM9" s="31">
+      <c r="AM9" s="30">
         <f t="shared" si="0"/>
         <v>42314</v>
       </c>
-      <c r="AN9" s="31">
+      <c r="AN9" s="30">
         <f t="shared" si="0"/>
         <v>42315</v>
       </c>
-      <c r="AO9" s="31">
+      <c r="AO9" s="30">
         <f t="shared" si="0"/>
         <v>42316</v>
       </c>
-      <c r="AP9" s="31">
+      <c r="AP9" s="30">
         <f t="shared" si="0"/>
         <v>42317</v>
       </c>
-      <c r="AQ9" s="31">
+      <c r="AQ9" s="30">
         <f t="shared" si="0"/>
         <v>42318</v>
       </c>
-      <c r="AR9" s="31">
+      <c r="AR9" s="30">
         <f t="shared" si="0"/>
         <v>42319</v>
       </c>
-      <c r="AS9" s="31">
+      <c r="AS9" s="30">
         <f t="shared" si="0"/>
         <v>42320</v>
       </c>
-      <c r="AT9" s="31">
+      <c r="AT9" s="30">
         <f t="shared" si="0"/>
         <v>42321</v>
       </c>
-      <c r="AU9" s="31">
+      <c r="AU9" s="30">
         <f t="shared" si="0"/>
         <v>42322</v>
       </c>
-      <c r="AV9" s="31">
+      <c r="AV9" s="30">
         <f t="shared" si="0"/>
         <v>42323</v>
       </c>
-      <c r="AW9" s="31">
+      <c r="AW9" s="30">
         <f t="shared" si="0"/>
         <v>42324</v>
       </c>
-      <c r="AX9" s="31">
+      <c r="AX9" s="30">
         <f t="shared" si="0"/>
         <v>42325</v>
       </c>
-      <c r="AY9" s="31">
+      <c r="AY9" s="30">
         <f t="shared" si="0"/>
         <v>42326</v>
       </c>
-      <c r="AZ9" s="31">
+      <c r="AZ9" s="30">
         <f t="shared" si="0"/>
         <v>42327</v>
       </c>
-      <c r="BA9" s="31">
+      <c r="BA9" s="30">
         <f t="shared" si="0"/>
         <v>42328</v>
       </c>
-      <c r="BB9" s="31">
+      <c r="BB9" s="30">
         <f t="shared" si="0"/>
         <v>42329</v>
       </c>
-      <c r="BC9" s="31">
+      <c r="BC9" s="30">
         <f t="shared" si="0"/>
         <v>42330</v>
       </c>
-      <c r="BD9" s="31">
+      <c r="BD9" s="30">
         <f t="shared" si="0"/>
         <v>42331</v>
       </c>
-      <c r="BE9" s="31">
+      <c r="BE9" s="30">
         <f t="shared" si="0"/>
         <v>42332</v>
       </c>
-      <c r="BF9" s="31">
+      <c r="BF9" s="30">
         <f t="shared" si="0"/>
         <v>42333</v>
       </c>
-      <c r="BG9" s="31">
+      <c r="BG9" s="30">
         <f t="shared" si="0"/>
         <v>42334</v>
       </c>
-      <c r="BH9" s="31">
+      <c r="BH9" s="30">
         <f t="shared" si="0"/>
         <v>42335</v>
       </c>
-      <c r="BI9" s="31">
+      <c r="BI9" s="30">
         <f t="shared" si="0"/>
         <v>42336</v>
       </c>
-      <c r="BJ9" s="31">
+      <c r="BJ9" s="30">
         <f t="shared" si="0"/>
         <v>42337</v>
       </c>
-      <c r="BK9" s="31">
+      <c r="BK9" s="30">
         <f t="shared" si="0"/>
         <v>42338</v>
       </c>
-      <c r="BL9" s="31">
+      <c r="BL9" s="30">
         <f t="shared" si="0"/>
         <v>42339</v>
       </c>
-      <c r="BM9" s="31">
+      <c r="BM9" s="30">
         <f t="shared" si="0"/>
         <v>42340</v>
       </c>
-      <c r="BN9" s="31">
+      <c r="BN9" s="30">
         <f t="shared" si="0"/>
         <v>42341</v>
       </c>
-      <c r="BO9" s="31">
+      <c r="BO9" s="30">
         <f t="shared" si="0"/>
         <v>42342</v>
       </c>
-      <c r="BP9" s="31">
+      <c r="BP9" s="30">
         <f t="shared" si="0"/>
         <v>42343</v>
       </c>
-      <c r="BQ9" s="31">
+      <c r="BQ9" s="30">
         <f t="shared" si="0"/>
         <v>42344</v>
       </c>
-      <c r="BR9" s="31">
+      <c r="BR9" s="30">
         <f t="shared" si="0"/>
         <v>42345</v>
       </c>
-      <c r="BS9" s="31">
+      <c r="BS9" s="30">
         <f t="shared" si="0"/>
         <v>42346</v>
       </c>
-      <c r="BT9" s="31">
+      <c r="BT9" s="30">
         <f t="shared" si="0"/>
         <v>42347</v>
       </c>
-      <c r="BU9" s="31">
+      <c r="BU9" s="30">
         <f t="shared" si="0"/>
         <v>42348</v>
       </c>
-      <c r="BV9" s="31">
+      <c r="BV9" s="30">
         <f t="shared" si="0"/>
         <v>42349</v>
       </c>
-      <c r="BW9" s="31">
-        <f t="shared" ref="BW9:CC9" si="1">BV9+1</f>
+      <c r="BW9" s="30">
+        <f t="shared" ref="BW9:BZ9" si="1">BV9+1</f>
         <v>42350</v>
       </c>
-      <c r="BX9" s="31">
+      <c r="BX9" s="30">
         <f t="shared" si="1"/>
         <v>42351</v>
       </c>
-      <c r="BY9" s="31">
+      <c r="BY9" s="30">
         <f t="shared" si="1"/>
         <v>42352</v>
       </c>
-      <c r="BZ9" s="31">
+      <c r="BZ9" s="30">
         <f t="shared" si="1"/>
         <v>42353</v>
       </c>
     </row>
-    <row r="10" spans="2:78" ht="15" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:109" ht="15" x14ac:dyDescent="0.25">
       <c r="B10" s="4"/>
       <c r="C10" s="4" t="s">
         <v>3</v>
@@ -1834,7 +1511,7 @@
       <c r="AU10" s="1"/>
       <c r="AV10" s="1"/>
     </row>
-    <row r="11" spans="2:78" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:109" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="5" t="s">
         <v>9</v>
       </c>
@@ -1859,7 +1536,7 @@
       </c>
       <c r="J11" s="4"/>
     </row>
-    <row r="12" spans="2:78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:109" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -2047,9 +1724,131 @@
       <c r="BP12" s="3">
         <v>60</v>
       </c>
-      <c r="BQ12" s="1"/>
+      <c r="BQ12" s="3">
+        <v>61</v>
+      </c>
+      <c r="BR12" s="3">
+        <v>62</v>
+      </c>
+      <c r="BS12" s="3">
+        <v>63</v>
+      </c>
+      <c r="BT12" s="3">
+        <v>64</v>
+      </c>
+      <c r="BU12" s="3">
+        <v>65</v>
+      </c>
+      <c r="BV12" s="3">
+        <v>66</v>
+      </c>
+      <c r="BW12" s="3">
+        <v>67</v>
+      </c>
+      <c r="BX12" s="3">
+        <v>68</v>
+      </c>
+      <c r="BY12" s="3">
+        <v>69</v>
+      </c>
+      <c r="BZ12" s="3">
+        <v>70</v>
+      </c>
+      <c r="CA12" s="3">
+        <v>71</v>
+      </c>
+      <c r="CB12" s="3">
+        <v>72</v>
+      </c>
+      <c r="CC12" s="3">
+        <v>73</v>
+      </c>
+      <c r="CD12" s="3">
+        <v>74</v>
+      </c>
+      <c r="CE12" s="3">
+        <v>75</v>
+      </c>
+      <c r="CF12" s="3">
+        <v>76</v>
+      </c>
+      <c r="CG12" s="3">
+        <v>77</v>
+      </c>
+      <c r="CH12" s="3">
+        <v>78</v>
+      </c>
+      <c r="CI12" s="3">
+        <v>79</v>
+      </c>
+      <c r="CJ12" s="3">
+        <v>80</v>
+      </c>
+      <c r="CK12" s="3">
+        <v>81</v>
+      </c>
+      <c r="CL12" s="3">
+        <v>82</v>
+      </c>
+      <c r="CM12" s="3">
+        <v>83</v>
+      </c>
+      <c r="CN12" s="3">
+        <v>84</v>
+      </c>
+      <c r="CO12" s="3">
+        <v>85</v>
+      </c>
+      <c r="CP12" s="3">
+        <v>86</v>
+      </c>
+      <c r="CQ12" s="3">
+        <v>87</v>
+      </c>
+      <c r="CR12" s="3">
+        <v>88</v>
+      </c>
+      <c r="CS12" s="3">
+        <v>89</v>
+      </c>
+      <c r="CT12" s="3">
+        <v>90</v>
+      </c>
+      <c r="CU12" s="3">
+        <v>91</v>
+      </c>
+      <c r="CV12" s="3">
+        <v>92</v>
+      </c>
+      <c r="CW12" s="3">
+        <v>93</v>
+      </c>
+      <c r="CX12" s="3">
+        <v>94</v>
+      </c>
+      <c r="CY12" s="3">
+        <v>95</v>
+      </c>
+      <c r="CZ12" s="3">
+        <v>96</v>
+      </c>
+      <c r="DA12" s="3">
+        <v>97</v>
+      </c>
+      <c r="DB12" s="3">
+        <v>98</v>
+      </c>
+      <c r="DC12" s="3">
+        <v>99</v>
+      </c>
+      <c r="DD12" s="3">
+        <v>100</v>
+      </c>
+      <c r="DE12" s="3">
+        <v>101</v>
+      </c>
     </row>
-    <row r="13" spans="2:78" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="s">
         <v>14</v>
       </c>
@@ -2057,7 +1856,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="16">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E13" s="16">
         <f>C13</f>
@@ -2065,95 +1864,129 @@
       </c>
       <c r="F13" s="16">
         <f>D13</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G13" s="17">
         <v>1</v>
       </c>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="32"/>
+      <c r="M13" s="32"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
     </row>
-    <row r="14" spans="2:78" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:109" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="15" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="16">
         <f>D13+C13</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D14" s="16">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E14" s="16">
         <f t="shared" ref="E14:E19" si="2">C14</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F14" s="16">
         <f t="shared" ref="F14:F19" si="3">D14</f>
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="G14" s="17">
-        <v>0.5</v>
-      </c>
+        <v>0.8</v>
+      </c>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="32"/>
+      <c r="T14" s="32"/>
+      <c r="U14" s="32"/>
+      <c r="V14" s="32"/>
+      <c r="W14" s="32"/>
+      <c r="X14" s="32"/>
+      <c r="Y14" s="32"/>
+      <c r="Z14" s="32"/>
+      <c r="AA14" s="32"/>
+      <c r="AB14" s="32"/>
+      <c r="AC14" s="32"/>
+      <c r="AD14" s="32"/>
+      <c r="AE14" s="32"/>
+      <c r="AF14" s="32"/>
+      <c r="AG14" s="32"/>
+      <c r="AH14" s="32"/>
+      <c r="AI14" s="32"/>
     </row>
-    <row r="15" spans="2:78" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="15" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="16">
         <f t="shared" ref="C15:C19" si="4">D14+C14</f>
+        <v>28</v>
+      </c>
+      <c r="D15" s="16">
         <v>10</v>
-      </c>
-      <c r="D15" s="16">
-        <v>7</v>
       </c>
       <c r="E15" s="16">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F15" s="16">
         <f t="shared" si="3"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G15" s="17">
         <v>0</v>
       </c>
+      <c r="AJ15" s="32"/>
+      <c r="AK15" s="32"/>
+      <c r="AL15" s="32"/>
+      <c r="AM15" s="32"/>
+      <c r="AN15" s="32"/>
+      <c r="AO15" s="32"/>
+      <c r="AP15" s="32"/>
     </row>
-    <row r="16" spans="2:78" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="15" t="s">
         <v>17</v>
       </c>
       <c r="C16" s="16">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="D16" s="16">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E16" s="16">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="F16" s="16">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G16" s="17">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="15" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="16">
         <f t="shared" si="4"/>
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="D17" s="16">
         <v>8</v>
       </c>
       <c r="E17" s="16">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="F17" s="16">
         <f t="shared" si="3"/>
@@ -2163,20 +1996,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="16">
         <f t="shared" si="4"/>
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="D18" s="16">
         <v>15</v>
       </c>
       <c r="E18" s="16">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="F18" s="16">
         <f t="shared" si="3"/>
@@ -2186,20 +2019,20 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C19" s="16">
         <f t="shared" si="4"/>
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="D19" s="16">
         <v>5</v>
       </c>
       <c r="E19" s="16">
         <f t="shared" si="2"/>
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="F19" s="16">
         <f t="shared" si="3"/>
@@ -2209,7 +2042,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="20" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
@@ -2277,8 +2110,49 @@
       <c r="BN20" s="19"/>
       <c r="BO20" s="19"/>
       <c r="BP20" s="19"/>
+      <c r="BQ20" s="19"/>
+      <c r="BR20" s="19"/>
+      <c r="BS20" s="19"/>
+      <c r="BT20" s="19"/>
+      <c r="BU20" s="19"/>
+      <c r="BV20" s="19"/>
+      <c r="BW20" s="19"/>
+      <c r="BX20" s="19"/>
+      <c r="BY20" s="19"/>
+      <c r="BZ20" s="19"/>
+      <c r="CA20" s="19"/>
+      <c r="CB20" s="19"/>
+      <c r="CC20" s="19"/>
+      <c r="CD20" s="19"/>
+      <c r="CE20" s="19"/>
+      <c r="CF20" s="19"/>
+      <c r="CG20" s="19"/>
+      <c r="CH20" s="19"/>
+      <c r="CI20" s="19"/>
+      <c r="CJ20" s="19"/>
+      <c r="CK20" s="19"/>
+      <c r="CL20" s="19"/>
+      <c r="CM20" s="19"/>
+      <c r="CN20" s="19"/>
+      <c r="CO20" s="19"/>
+      <c r="CP20" s="19"/>
+      <c r="CQ20" s="19"/>
+      <c r="CR20" s="19"/>
+      <c r="CS20" s="19"/>
+      <c r="CT20" s="19"/>
+      <c r="CU20" s="19"/>
+      <c r="CV20" s="19"/>
+      <c r="CW20" s="19"/>
+      <c r="CX20" s="19"/>
+      <c r="CY20" s="19"/>
+      <c r="CZ20" s="19"/>
+      <c r="DA20" s="19"/>
+      <c r="DB20" s="19"/>
+      <c r="DC20" s="19"/>
+      <c r="DD20" s="19"/>
+      <c r="DE20" s="19"/>
     </row>
-    <row r="21" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
@@ -2346,8 +2220,49 @@
       <c r="BN21" s="19"/>
       <c r="BO21" s="19"/>
       <c r="BP21" s="19"/>
+      <c r="BQ21" s="19"/>
+      <c r="BR21" s="19"/>
+      <c r="BS21" s="19"/>
+      <c r="BT21" s="19"/>
+      <c r="BU21" s="19"/>
+      <c r="BV21" s="19"/>
+      <c r="BW21" s="19"/>
+      <c r="BX21" s="19"/>
+      <c r="BY21" s="19"/>
+      <c r="BZ21" s="19"/>
+      <c r="CA21" s="19"/>
+      <c r="CB21" s="19"/>
+      <c r="CC21" s="19"/>
+      <c r="CD21" s="19"/>
+      <c r="CE21" s="19"/>
+      <c r="CF21" s="19"/>
+      <c r="CG21" s="19"/>
+      <c r="CH21" s="19"/>
+      <c r="CI21" s="19"/>
+      <c r="CJ21" s="19"/>
+      <c r="CK21" s="19"/>
+      <c r="CL21" s="19"/>
+      <c r="CM21" s="19"/>
+      <c r="CN21" s="19"/>
+      <c r="CO21" s="19"/>
+      <c r="CP21" s="19"/>
+      <c r="CQ21" s="19"/>
+      <c r="CR21" s="19"/>
+      <c r="CS21" s="19"/>
+      <c r="CT21" s="19"/>
+      <c r="CU21" s="19"/>
+      <c r="CV21" s="19"/>
+      <c r="CW21" s="19"/>
+      <c r="CX21" s="19"/>
+      <c r="CY21" s="19"/>
+      <c r="CZ21" s="19"/>
+      <c r="DA21" s="19"/>
+      <c r="DB21" s="19"/>
+      <c r="DC21" s="19"/>
+      <c r="DD21" s="19"/>
+      <c r="DE21" s="19"/>
     </row>
-    <row r="22" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
@@ -2415,8 +2330,49 @@
       <c r="BN22" s="19"/>
       <c r="BO22" s="19"/>
       <c r="BP22" s="19"/>
+      <c r="BQ22" s="19"/>
+      <c r="BR22" s="19"/>
+      <c r="BS22" s="19"/>
+      <c r="BT22" s="19"/>
+      <c r="BU22" s="19"/>
+      <c r="BV22" s="19"/>
+      <c r="BW22" s="19"/>
+      <c r="BX22" s="19"/>
+      <c r="BY22" s="19"/>
+      <c r="BZ22" s="19"/>
+      <c r="CA22" s="19"/>
+      <c r="CB22" s="19"/>
+      <c r="CC22" s="19"/>
+      <c r="CD22" s="19"/>
+      <c r="CE22" s="19"/>
+      <c r="CF22" s="19"/>
+      <c r="CG22" s="19"/>
+      <c r="CH22" s="19"/>
+      <c r="CI22" s="19"/>
+      <c r="CJ22" s="19"/>
+      <c r="CK22" s="19"/>
+      <c r="CL22" s="19"/>
+      <c r="CM22" s="19"/>
+      <c r="CN22" s="19"/>
+      <c r="CO22" s="19"/>
+      <c r="CP22" s="19"/>
+      <c r="CQ22" s="19"/>
+      <c r="CR22" s="19"/>
+      <c r="CS22" s="19"/>
+      <c r="CT22" s="19"/>
+      <c r="CU22" s="19"/>
+      <c r="CV22" s="19"/>
+      <c r="CW22" s="19"/>
+      <c r="CX22" s="19"/>
+      <c r="CY22" s="19"/>
+      <c r="CZ22" s="19"/>
+      <c r="DA22" s="19"/>
+      <c r="DB22" s="19"/>
+      <c r="DC22" s="19"/>
+      <c r="DD22" s="19"/>
+      <c r="DE22" s="19"/>
     </row>
-    <row r="23" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="19"/>
       <c r="C23" s="19"/>
       <c r="D23" s="19"/>
@@ -2484,8 +2440,49 @@
       <c r="BN23" s="19"/>
       <c r="BO23" s="19"/>
       <c r="BP23" s="19"/>
+      <c r="BQ23" s="19"/>
+      <c r="BR23" s="19"/>
+      <c r="BS23" s="19"/>
+      <c r="BT23" s="19"/>
+      <c r="BU23" s="19"/>
+      <c r="BV23" s="19"/>
+      <c r="BW23" s="19"/>
+      <c r="BX23" s="19"/>
+      <c r="BY23" s="19"/>
+      <c r="BZ23" s="19"/>
+      <c r="CA23" s="19"/>
+      <c r="CB23" s="19"/>
+      <c r="CC23" s="19"/>
+      <c r="CD23" s="19"/>
+      <c r="CE23" s="19"/>
+      <c r="CF23" s="19"/>
+      <c r="CG23" s="19"/>
+      <c r="CH23" s="19"/>
+      <c r="CI23" s="19"/>
+      <c r="CJ23" s="19"/>
+      <c r="CK23" s="19"/>
+      <c r="CL23" s="19"/>
+      <c r="CM23" s="19"/>
+      <c r="CN23" s="19"/>
+      <c r="CO23" s="19"/>
+      <c r="CP23" s="19"/>
+      <c r="CQ23" s="19"/>
+      <c r="CR23" s="19"/>
+      <c r="CS23" s="19"/>
+      <c r="CT23" s="19"/>
+      <c r="CU23" s="19"/>
+      <c r="CV23" s="19"/>
+      <c r="CW23" s="19"/>
+      <c r="CX23" s="19"/>
+      <c r="CY23" s="19"/>
+      <c r="CZ23" s="19"/>
+      <c r="DA23" s="19"/>
+      <c r="DB23" s="19"/>
+      <c r="DC23" s="19"/>
+      <c r="DD23" s="19"/>
+      <c r="DE23" s="19"/>
     </row>
-    <row r="24" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="19"/>
       <c r="C24" s="21"/>
       <c r="D24" s="19"/>
@@ -2553,8 +2550,49 @@
       <c r="BN24" s="19"/>
       <c r="BO24" s="19"/>
       <c r="BP24" s="19"/>
+      <c r="BQ24" s="19"/>
+      <c r="BR24" s="19"/>
+      <c r="BS24" s="19"/>
+      <c r="BT24" s="19"/>
+      <c r="BU24" s="19"/>
+      <c r="BV24" s="19"/>
+      <c r="BW24" s="19"/>
+      <c r="BX24" s="19"/>
+      <c r="BY24" s="19"/>
+      <c r="BZ24" s="19"/>
+      <c r="CA24" s="19"/>
+      <c r="CB24" s="19"/>
+      <c r="CC24" s="19"/>
+      <c r="CD24" s="19"/>
+      <c r="CE24" s="19"/>
+      <c r="CF24" s="19"/>
+      <c r="CG24" s="19"/>
+      <c r="CH24" s="19"/>
+      <c r="CI24" s="19"/>
+      <c r="CJ24" s="19"/>
+      <c r="CK24" s="19"/>
+      <c r="CL24" s="19"/>
+      <c r="CM24" s="19"/>
+      <c r="CN24" s="19"/>
+      <c r="CO24" s="19"/>
+      <c r="CP24" s="19"/>
+      <c r="CQ24" s="19"/>
+      <c r="CR24" s="19"/>
+      <c r="CS24" s="19"/>
+      <c r="CT24" s="19"/>
+      <c r="CU24" s="19"/>
+      <c r="CV24" s="19"/>
+      <c r="CW24" s="19"/>
+      <c r="CX24" s="19"/>
+      <c r="CY24" s="19"/>
+      <c r="CZ24" s="19"/>
+      <c r="DA24" s="19"/>
+      <c r="DB24" s="19"/>
+      <c r="DC24" s="19"/>
+      <c r="DD24" s="19"/>
+      <c r="DE24" s="19"/>
     </row>
-    <row r="25" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="19"/>
       <c r="C25" s="19"/>
       <c r="D25" s="19"/>
@@ -2622,8 +2660,49 @@
       <c r="BN25" s="19"/>
       <c r="BO25" s="19"/>
       <c r="BP25" s="19"/>
+      <c r="BQ25" s="19"/>
+      <c r="BR25" s="19"/>
+      <c r="BS25" s="19"/>
+      <c r="BT25" s="19"/>
+      <c r="BU25" s="19"/>
+      <c r="BV25" s="19"/>
+      <c r="BW25" s="19"/>
+      <c r="BX25" s="19"/>
+      <c r="BY25" s="19"/>
+      <c r="BZ25" s="19"/>
+      <c r="CA25" s="19"/>
+      <c r="CB25" s="19"/>
+      <c r="CC25" s="19"/>
+      <c r="CD25" s="19"/>
+      <c r="CE25" s="19"/>
+      <c r="CF25" s="19"/>
+      <c r="CG25" s="19"/>
+      <c r="CH25" s="19"/>
+      <c r="CI25" s="19"/>
+      <c r="CJ25" s="19"/>
+      <c r="CK25" s="19"/>
+      <c r="CL25" s="19"/>
+      <c r="CM25" s="19"/>
+      <c r="CN25" s="19"/>
+      <c r="CO25" s="19"/>
+      <c r="CP25" s="19"/>
+      <c r="CQ25" s="19"/>
+      <c r="CR25" s="19"/>
+      <c r="CS25" s="19"/>
+      <c r="CT25" s="19"/>
+      <c r="CU25" s="19"/>
+      <c r="CV25" s="19"/>
+      <c r="CW25" s="19"/>
+      <c r="CX25" s="19"/>
+      <c r="CY25" s="19"/>
+      <c r="CZ25" s="19"/>
+      <c r="DA25" s="19"/>
+      <c r="DB25" s="19"/>
+      <c r="DC25" s="19"/>
+      <c r="DD25" s="19"/>
+      <c r="DE25" s="19"/>
     </row>
-    <row r="26" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
       <c r="D26" s="19"/>
@@ -2691,8 +2770,49 @@
       <c r="BN26" s="19"/>
       <c r="BO26" s="19"/>
       <c r="BP26" s="19"/>
+      <c r="BQ26" s="19"/>
+      <c r="BR26" s="19"/>
+      <c r="BS26" s="19"/>
+      <c r="BT26" s="19"/>
+      <c r="BU26" s="19"/>
+      <c r="BV26" s="19"/>
+      <c r="BW26" s="19"/>
+      <c r="BX26" s="19"/>
+      <c r="BY26" s="19"/>
+      <c r="BZ26" s="19"/>
+      <c r="CA26" s="19"/>
+      <c r="CB26" s="19"/>
+      <c r="CC26" s="19"/>
+      <c r="CD26" s="19"/>
+      <c r="CE26" s="19"/>
+      <c r="CF26" s="19"/>
+      <c r="CG26" s="19"/>
+      <c r="CH26" s="19"/>
+      <c r="CI26" s="19"/>
+      <c r="CJ26" s="19"/>
+      <c r="CK26" s="19"/>
+      <c r="CL26" s="19"/>
+      <c r="CM26" s="19"/>
+      <c r="CN26" s="19"/>
+      <c r="CO26" s="19"/>
+      <c r="CP26" s="19"/>
+      <c r="CQ26" s="19"/>
+      <c r="CR26" s="19"/>
+      <c r="CS26" s="19"/>
+      <c r="CT26" s="19"/>
+      <c r="CU26" s="19"/>
+      <c r="CV26" s="19"/>
+      <c r="CW26" s="19"/>
+      <c r="CX26" s="19"/>
+      <c r="CY26" s="19"/>
+      <c r="CZ26" s="19"/>
+      <c r="DA26" s="19"/>
+      <c r="DB26" s="19"/>
+      <c r="DC26" s="19"/>
+      <c r="DD26" s="19"/>
+      <c r="DE26" s="19"/>
     </row>
-    <row r="27" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="19"/>
       <c r="C27" s="19"/>
       <c r="D27" s="19"/>
@@ -2760,8 +2880,49 @@
       <c r="BN27" s="19"/>
       <c r="BO27" s="19"/>
       <c r="BP27" s="19"/>
+      <c r="BQ27" s="19"/>
+      <c r="BR27" s="19"/>
+      <c r="BS27" s="19"/>
+      <c r="BT27" s="19"/>
+      <c r="BU27" s="19"/>
+      <c r="BV27" s="19"/>
+      <c r="BW27" s="19"/>
+      <c r="BX27" s="19"/>
+      <c r="BY27" s="19"/>
+      <c r="BZ27" s="19"/>
+      <c r="CA27" s="19"/>
+      <c r="CB27" s="19"/>
+      <c r="CC27" s="19"/>
+      <c r="CD27" s="19"/>
+      <c r="CE27" s="19"/>
+      <c r="CF27" s="19"/>
+      <c r="CG27" s="19"/>
+      <c r="CH27" s="19"/>
+      <c r="CI27" s="19"/>
+      <c r="CJ27" s="19"/>
+      <c r="CK27" s="19"/>
+      <c r="CL27" s="19"/>
+      <c r="CM27" s="19"/>
+      <c r="CN27" s="19"/>
+      <c r="CO27" s="19"/>
+      <c r="CP27" s="19"/>
+      <c r="CQ27" s="19"/>
+      <c r="CR27" s="19"/>
+      <c r="CS27" s="19"/>
+      <c r="CT27" s="19"/>
+      <c r="CU27" s="19"/>
+      <c r="CV27" s="19"/>
+      <c r="CW27" s="19"/>
+      <c r="CX27" s="19"/>
+      <c r="CY27" s="19"/>
+      <c r="CZ27" s="19"/>
+      <c r="DA27" s="19"/>
+      <c r="DB27" s="19"/>
+      <c r="DC27" s="19"/>
+      <c r="DD27" s="19"/>
+      <c r="DE27" s="19"/>
     </row>
-    <row r="28" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="19"/>
       <c r="C28" s="19"/>
       <c r="D28" s="19"/>
@@ -2829,8 +2990,49 @@
       <c r="BN28" s="19"/>
       <c r="BO28" s="19"/>
       <c r="BP28" s="19"/>
+      <c r="BQ28" s="19"/>
+      <c r="BR28" s="19"/>
+      <c r="BS28" s="19"/>
+      <c r="BT28" s="19"/>
+      <c r="BU28" s="19"/>
+      <c r="BV28" s="19"/>
+      <c r="BW28" s="19"/>
+      <c r="BX28" s="19"/>
+      <c r="BY28" s="19"/>
+      <c r="BZ28" s="19"/>
+      <c r="CA28" s="19"/>
+      <c r="CB28" s="19"/>
+      <c r="CC28" s="19"/>
+      <c r="CD28" s="19"/>
+      <c r="CE28" s="19"/>
+      <c r="CF28" s="19"/>
+      <c r="CG28" s="19"/>
+      <c r="CH28" s="19"/>
+      <c r="CI28" s="19"/>
+      <c r="CJ28" s="19"/>
+      <c r="CK28" s="19"/>
+      <c r="CL28" s="19"/>
+      <c r="CM28" s="19"/>
+      <c r="CN28" s="19"/>
+      <c r="CO28" s="19"/>
+      <c r="CP28" s="19"/>
+      <c r="CQ28" s="19"/>
+      <c r="CR28" s="19"/>
+      <c r="CS28" s="19"/>
+      <c r="CT28" s="19"/>
+      <c r="CU28" s="19"/>
+      <c r="CV28" s="19"/>
+      <c r="CW28" s="19"/>
+      <c r="CX28" s="19"/>
+      <c r="CY28" s="19"/>
+      <c r="CZ28" s="19"/>
+      <c r="DA28" s="19"/>
+      <c r="DB28" s="19"/>
+      <c r="DC28" s="19"/>
+      <c r="DD28" s="19"/>
+      <c r="DE28" s="19"/>
     </row>
-    <row r="29" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="19"/>
       <c r="C29" s="19"/>
       <c r="D29" s="19"/>
@@ -2898,8 +3100,49 @@
       <c r="BN29" s="19"/>
       <c r="BO29" s="19"/>
       <c r="BP29" s="19"/>
+      <c r="BQ29" s="19"/>
+      <c r="BR29" s="19"/>
+      <c r="BS29" s="19"/>
+      <c r="BT29" s="19"/>
+      <c r="BU29" s="19"/>
+      <c r="BV29" s="19"/>
+      <c r="BW29" s="19"/>
+      <c r="BX29" s="19"/>
+      <c r="BY29" s="19"/>
+      <c r="BZ29" s="19"/>
+      <c r="CA29" s="19"/>
+      <c r="CB29" s="19"/>
+      <c r="CC29" s="19"/>
+      <c r="CD29" s="19"/>
+      <c r="CE29" s="19"/>
+      <c r="CF29" s="19"/>
+      <c r="CG29" s="19"/>
+      <c r="CH29" s="19"/>
+      <c r="CI29" s="19"/>
+      <c r="CJ29" s="19"/>
+      <c r="CK29" s="19"/>
+      <c r="CL29" s="19"/>
+      <c r="CM29" s="19"/>
+      <c r="CN29" s="19"/>
+      <c r="CO29" s="19"/>
+      <c r="CP29" s="19"/>
+      <c r="CQ29" s="19"/>
+      <c r="CR29" s="19"/>
+      <c r="CS29" s="19"/>
+      <c r="CT29" s="19"/>
+      <c r="CU29" s="19"/>
+      <c r="CV29" s="19"/>
+      <c r="CW29" s="19"/>
+      <c r="CX29" s="19"/>
+      <c r="CY29" s="19"/>
+      <c r="CZ29" s="19"/>
+      <c r="DA29" s="19"/>
+      <c r="DB29" s="19"/>
+      <c r="DC29" s="19"/>
+      <c r="DD29" s="19"/>
+      <c r="DE29" s="19"/>
     </row>
-    <row r="30" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="19"/>
       <c r="C30" s="19"/>
       <c r="D30" s="19"/>
@@ -2967,8 +3210,49 @@
       <c r="BN30" s="19"/>
       <c r="BO30" s="19"/>
       <c r="BP30" s="19"/>
+      <c r="BQ30" s="19"/>
+      <c r="BR30" s="19"/>
+      <c r="BS30" s="19"/>
+      <c r="BT30" s="19"/>
+      <c r="BU30" s="19"/>
+      <c r="BV30" s="19"/>
+      <c r="BW30" s="19"/>
+      <c r="BX30" s="19"/>
+      <c r="BY30" s="19"/>
+      <c r="BZ30" s="19"/>
+      <c r="CA30" s="19"/>
+      <c r="CB30" s="19"/>
+      <c r="CC30" s="19"/>
+      <c r="CD30" s="19"/>
+      <c r="CE30" s="19"/>
+      <c r="CF30" s="19"/>
+      <c r="CG30" s="19"/>
+      <c r="CH30" s="19"/>
+      <c r="CI30" s="19"/>
+      <c r="CJ30" s="19"/>
+      <c r="CK30" s="19"/>
+      <c r="CL30" s="19"/>
+      <c r="CM30" s="19"/>
+      <c r="CN30" s="19"/>
+      <c r="CO30" s="19"/>
+      <c r="CP30" s="19"/>
+      <c r="CQ30" s="19"/>
+      <c r="CR30" s="19"/>
+      <c r="CS30" s="19"/>
+      <c r="CT30" s="19"/>
+      <c r="CU30" s="19"/>
+      <c r="CV30" s="19"/>
+      <c r="CW30" s="19"/>
+      <c r="CX30" s="19"/>
+      <c r="CY30" s="19"/>
+      <c r="CZ30" s="19"/>
+      <c r="DA30" s="19"/>
+      <c r="DB30" s="19"/>
+      <c r="DC30" s="19"/>
+      <c r="DD30" s="19"/>
+      <c r="DE30" s="19"/>
     </row>
-    <row r="31" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="19"/>
       <c r="C31" s="19"/>
       <c r="D31" s="19"/>
@@ -3036,8 +3320,49 @@
       <c r="BN31" s="19"/>
       <c r="BO31" s="19"/>
       <c r="BP31" s="19"/>
+      <c r="BQ31" s="19"/>
+      <c r="BR31" s="19"/>
+      <c r="BS31" s="19"/>
+      <c r="BT31" s="19"/>
+      <c r="BU31" s="19"/>
+      <c r="BV31" s="19"/>
+      <c r="BW31" s="19"/>
+      <c r="BX31" s="19"/>
+      <c r="BY31" s="19"/>
+      <c r="BZ31" s="19"/>
+      <c r="CA31" s="19"/>
+      <c r="CB31" s="19"/>
+      <c r="CC31" s="19"/>
+      <c r="CD31" s="19"/>
+      <c r="CE31" s="19"/>
+      <c r="CF31" s="19"/>
+      <c r="CG31" s="19"/>
+      <c r="CH31" s="19"/>
+      <c r="CI31" s="19"/>
+      <c r="CJ31" s="19"/>
+      <c r="CK31" s="19"/>
+      <c r="CL31" s="19"/>
+      <c r="CM31" s="19"/>
+      <c r="CN31" s="19"/>
+      <c r="CO31" s="19"/>
+      <c r="CP31" s="19"/>
+      <c r="CQ31" s="19"/>
+      <c r="CR31" s="19"/>
+      <c r="CS31" s="19"/>
+      <c r="CT31" s="19"/>
+      <c r="CU31" s="19"/>
+      <c r="CV31" s="19"/>
+      <c r="CW31" s="19"/>
+      <c r="CX31" s="19"/>
+      <c r="CY31" s="19"/>
+      <c r="CZ31" s="19"/>
+      <c r="DA31" s="19"/>
+      <c r="DB31" s="19"/>
+      <c r="DC31" s="19"/>
+      <c r="DD31" s="19"/>
+      <c r="DE31" s="19"/>
     </row>
-    <row r="32" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="19"/>
       <c r="C32" s="19"/>
       <c r="D32" s="19"/>
@@ -3105,8 +3430,49 @@
       <c r="BN32" s="19"/>
       <c r="BO32" s="19"/>
       <c r="BP32" s="19"/>
+      <c r="BQ32" s="19"/>
+      <c r="BR32" s="19"/>
+      <c r="BS32" s="19"/>
+      <c r="BT32" s="19"/>
+      <c r="BU32" s="19"/>
+      <c r="BV32" s="19"/>
+      <c r="BW32" s="19"/>
+      <c r="BX32" s="19"/>
+      <c r="BY32" s="19"/>
+      <c r="BZ32" s="19"/>
+      <c r="CA32" s="19"/>
+      <c r="CB32" s="19"/>
+      <c r="CC32" s="19"/>
+      <c r="CD32" s="19"/>
+      <c r="CE32" s="19"/>
+      <c r="CF32" s="19"/>
+      <c r="CG32" s="19"/>
+      <c r="CH32" s="19"/>
+      <c r="CI32" s="19"/>
+      <c r="CJ32" s="19"/>
+      <c r="CK32" s="19"/>
+      <c r="CL32" s="19"/>
+      <c r="CM32" s="19"/>
+      <c r="CN32" s="19"/>
+      <c r="CO32" s="19"/>
+      <c r="CP32" s="19"/>
+      <c r="CQ32" s="19"/>
+      <c r="CR32" s="19"/>
+      <c r="CS32" s="19"/>
+      <c r="CT32" s="19"/>
+      <c r="CU32" s="19"/>
+      <c r="CV32" s="19"/>
+      <c r="CW32" s="19"/>
+      <c r="CX32" s="19"/>
+      <c r="CY32" s="19"/>
+      <c r="CZ32" s="19"/>
+      <c r="DA32" s="19"/>
+      <c r="DB32" s="19"/>
+      <c r="DC32" s="19"/>
+      <c r="DD32" s="19"/>
+      <c r="DE32" s="19"/>
     </row>
-    <row r="33" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="19"/>
       <c r="C33" s="19"/>
       <c r="D33" s="19"/>
@@ -3174,8 +3540,49 @@
       <c r="BN33" s="19"/>
       <c r="BO33" s="19"/>
       <c r="BP33" s="19"/>
+      <c r="BQ33" s="19"/>
+      <c r="BR33" s="19"/>
+      <c r="BS33" s="19"/>
+      <c r="BT33" s="19"/>
+      <c r="BU33" s="19"/>
+      <c r="BV33" s="19"/>
+      <c r="BW33" s="19"/>
+      <c r="BX33" s="19"/>
+      <c r="BY33" s="19"/>
+      <c r="BZ33" s="19"/>
+      <c r="CA33" s="19"/>
+      <c r="CB33" s="19"/>
+      <c r="CC33" s="19"/>
+      <c r="CD33" s="19"/>
+      <c r="CE33" s="19"/>
+      <c r="CF33" s="19"/>
+      <c r="CG33" s="19"/>
+      <c r="CH33" s="19"/>
+      <c r="CI33" s="19"/>
+      <c r="CJ33" s="19"/>
+      <c r="CK33" s="19"/>
+      <c r="CL33" s="19"/>
+      <c r="CM33" s="19"/>
+      <c r="CN33" s="19"/>
+      <c r="CO33" s="19"/>
+      <c r="CP33" s="19"/>
+      <c r="CQ33" s="19"/>
+      <c r="CR33" s="19"/>
+      <c r="CS33" s="19"/>
+      <c r="CT33" s="19"/>
+      <c r="CU33" s="19"/>
+      <c r="CV33" s="19"/>
+      <c r="CW33" s="19"/>
+      <c r="CX33" s="19"/>
+      <c r="CY33" s="19"/>
+      <c r="CZ33" s="19"/>
+      <c r="DA33" s="19"/>
+      <c r="DB33" s="19"/>
+      <c r="DC33" s="19"/>
+      <c r="DD33" s="19"/>
+      <c r="DE33" s="19"/>
     </row>
-    <row r="34" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="19"/>
       <c r="C34" s="19"/>
       <c r="D34" s="19"/>
@@ -3243,8 +3650,49 @@
       <c r="BN34" s="19"/>
       <c r="BO34" s="19"/>
       <c r="BP34" s="19"/>
+      <c r="BQ34" s="19"/>
+      <c r="BR34" s="19"/>
+      <c r="BS34" s="19"/>
+      <c r="BT34" s="19"/>
+      <c r="BU34" s="19"/>
+      <c r="BV34" s="19"/>
+      <c r="BW34" s="19"/>
+      <c r="BX34" s="19"/>
+      <c r="BY34" s="19"/>
+      <c r="BZ34" s="19"/>
+      <c r="CA34" s="19"/>
+      <c r="CB34" s="19"/>
+      <c r="CC34" s="19"/>
+      <c r="CD34" s="19"/>
+      <c r="CE34" s="19"/>
+      <c r="CF34" s="19"/>
+      <c r="CG34" s="19"/>
+      <c r="CH34" s="19"/>
+      <c r="CI34" s="19"/>
+      <c r="CJ34" s="19"/>
+      <c r="CK34" s="19"/>
+      <c r="CL34" s="19"/>
+      <c r="CM34" s="19"/>
+      <c r="CN34" s="19"/>
+      <c r="CO34" s="19"/>
+      <c r="CP34" s="19"/>
+      <c r="CQ34" s="19"/>
+      <c r="CR34" s="19"/>
+      <c r="CS34" s="19"/>
+      <c r="CT34" s="19"/>
+      <c r="CU34" s="19"/>
+      <c r="CV34" s="19"/>
+      <c r="CW34" s="19"/>
+      <c r="CX34" s="19"/>
+      <c r="CY34" s="19"/>
+      <c r="CZ34" s="19"/>
+      <c r="DA34" s="19"/>
+      <c r="DB34" s="19"/>
+      <c r="DC34" s="19"/>
+      <c r="DD34" s="19"/>
+      <c r="DE34" s="19"/>
     </row>
-    <row r="35" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="19"/>
       <c r="C35" s="19"/>
       <c r="D35" s="19"/>
@@ -3312,8 +3760,49 @@
       <c r="BN35" s="19"/>
       <c r="BO35" s="19"/>
       <c r="BP35" s="19"/>
+      <c r="BQ35" s="19"/>
+      <c r="BR35" s="19"/>
+      <c r="BS35" s="19"/>
+      <c r="BT35" s="19"/>
+      <c r="BU35" s="19"/>
+      <c r="BV35" s="19"/>
+      <c r="BW35" s="19"/>
+      <c r="BX35" s="19"/>
+      <c r="BY35" s="19"/>
+      <c r="BZ35" s="19"/>
+      <c r="CA35" s="19"/>
+      <c r="CB35" s="19"/>
+      <c r="CC35" s="19"/>
+      <c r="CD35" s="19"/>
+      <c r="CE35" s="19"/>
+      <c r="CF35" s="19"/>
+      <c r="CG35" s="19"/>
+      <c r="CH35" s="19"/>
+      <c r="CI35" s="19"/>
+      <c r="CJ35" s="19"/>
+      <c r="CK35" s="19"/>
+      <c r="CL35" s="19"/>
+      <c r="CM35" s="19"/>
+      <c r="CN35" s="19"/>
+      <c r="CO35" s="19"/>
+      <c r="CP35" s="19"/>
+      <c r="CQ35" s="19"/>
+      <c r="CR35" s="19"/>
+      <c r="CS35" s="19"/>
+      <c r="CT35" s="19"/>
+      <c r="CU35" s="19"/>
+      <c r="CV35" s="19"/>
+      <c r="CW35" s="19"/>
+      <c r="CX35" s="19"/>
+      <c r="CY35" s="19"/>
+      <c r="CZ35" s="19"/>
+      <c r="DA35" s="19"/>
+      <c r="DB35" s="19"/>
+      <c r="DC35" s="19"/>
+      <c r="DD35" s="19"/>
+      <c r="DE35" s="19"/>
     </row>
-    <row r="36" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="19"/>
       <c r="C36" s="19"/>
       <c r="D36" s="19"/>
@@ -3381,8 +3870,49 @@
       <c r="BN36" s="19"/>
       <c r="BO36" s="19"/>
       <c r="BP36" s="19"/>
+      <c r="BQ36" s="19"/>
+      <c r="BR36" s="19"/>
+      <c r="BS36" s="19"/>
+      <c r="BT36" s="19"/>
+      <c r="BU36" s="19"/>
+      <c r="BV36" s="19"/>
+      <c r="BW36" s="19"/>
+      <c r="BX36" s="19"/>
+      <c r="BY36" s="19"/>
+      <c r="BZ36" s="19"/>
+      <c r="CA36" s="19"/>
+      <c r="CB36" s="19"/>
+      <c r="CC36" s="19"/>
+      <c r="CD36" s="19"/>
+      <c r="CE36" s="19"/>
+      <c r="CF36" s="19"/>
+      <c r="CG36" s="19"/>
+      <c r="CH36" s="19"/>
+      <c r="CI36" s="19"/>
+      <c r="CJ36" s="19"/>
+      <c r="CK36" s="19"/>
+      <c r="CL36" s="19"/>
+      <c r="CM36" s="19"/>
+      <c r="CN36" s="19"/>
+      <c r="CO36" s="19"/>
+      <c r="CP36" s="19"/>
+      <c r="CQ36" s="19"/>
+      <c r="CR36" s="19"/>
+      <c r="CS36" s="19"/>
+      <c r="CT36" s="19"/>
+      <c r="CU36" s="19"/>
+      <c r="CV36" s="19"/>
+      <c r="CW36" s="19"/>
+      <c r="CX36" s="19"/>
+      <c r="CY36" s="19"/>
+      <c r="CZ36" s="19"/>
+      <c r="DA36" s="19"/>
+      <c r="DB36" s="19"/>
+      <c r="DC36" s="19"/>
+      <c r="DD36" s="19"/>
+      <c r="DE36" s="19"/>
     </row>
-    <row r="37" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="19"/>
       <c r="C37" s="19"/>
       <c r="D37" s="19"/>
@@ -3450,8 +3980,49 @@
       <c r="BN37" s="19"/>
       <c r="BO37" s="19"/>
       <c r="BP37" s="19"/>
+      <c r="BQ37" s="19"/>
+      <c r="BR37" s="19"/>
+      <c r="BS37" s="19"/>
+      <c r="BT37" s="19"/>
+      <c r="BU37" s="19"/>
+      <c r="BV37" s="19"/>
+      <c r="BW37" s="19"/>
+      <c r="BX37" s="19"/>
+      <c r="BY37" s="19"/>
+      <c r="BZ37" s="19"/>
+      <c r="CA37" s="19"/>
+      <c r="CB37" s="19"/>
+      <c r="CC37" s="19"/>
+      <c r="CD37" s="19"/>
+      <c r="CE37" s="19"/>
+      <c r="CF37" s="19"/>
+      <c r="CG37" s="19"/>
+      <c r="CH37" s="19"/>
+      <c r="CI37" s="19"/>
+      <c r="CJ37" s="19"/>
+      <c r="CK37" s="19"/>
+      <c r="CL37" s="19"/>
+      <c r="CM37" s="19"/>
+      <c r="CN37" s="19"/>
+      <c r="CO37" s="19"/>
+      <c r="CP37" s="19"/>
+      <c r="CQ37" s="19"/>
+      <c r="CR37" s="19"/>
+      <c r="CS37" s="19"/>
+      <c r="CT37" s="19"/>
+      <c r="CU37" s="19"/>
+      <c r="CV37" s="19"/>
+      <c r="CW37" s="19"/>
+      <c r="CX37" s="19"/>
+      <c r="CY37" s="19"/>
+      <c r="CZ37" s="19"/>
+      <c r="DA37" s="19"/>
+      <c r="DB37" s="19"/>
+      <c r="DC37" s="19"/>
+      <c r="DD37" s="19"/>
+      <c r="DE37" s="19"/>
     </row>
-    <row r="38" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="19"/>
       <c r="C38" s="19"/>
       <c r="D38" s="19"/>
@@ -3519,8 +4090,49 @@
       <c r="BN38" s="19"/>
       <c r="BO38" s="19"/>
       <c r="BP38" s="19"/>
+      <c r="BQ38" s="19"/>
+      <c r="BR38" s="19"/>
+      <c r="BS38" s="19"/>
+      <c r="BT38" s="19"/>
+      <c r="BU38" s="19"/>
+      <c r="BV38" s="19"/>
+      <c r="BW38" s="19"/>
+      <c r="BX38" s="19"/>
+      <c r="BY38" s="19"/>
+      <c r="BZ38" s="19"/>
+      <c r="CA38" s="19"/>
+      <c r="CB38" s="19"/>
+      <c r="CC38" s="19"/>
+      <c r="CD38" s="19"/>
+      <c r="CE38" s="19"/>
+      <c r="CF38" s="19"/>
+      <c r="CG38" s="19"/>
+      <c r="CH38" s="19"/>
+      <c r="CI38" s="19"/>
+      <c r="CJ38" s="19"/>
+      <c r="CK38" s="19"/>
+      <c r="CL38" s="19"/>
+      <c r="CM38" s="19"/>
+      <c r="CN38" s="19"/>
+      <c r="CO38" s="19"/>
+      <c r="CP38" s="19"/>
+      <c r="CQ38" s="19"/>
+      <c r="CR38" s="19"/>
+      <c r="CS38" s="19"/>
+      <c r="CT38" s="19"/>
+      <c r="CU38" s="19"/>
+      <c r="CV38" s="19"/>
+      <c r="CW38" s="19"/>
+      <c r="CX38" s="19"/>
+      <c r="CY38" s="19"/>
+      <c r="CZ38" s="19"/>
+      <c r="DA38" s="19"/>
+      <c r="DB38" s="19"/>
+      <c r="DC38" s="19"/>
+      <c r="DD38" s="19"/>
+      <c r="DE38" s="19"/>
     </row>
-    <row r="39" spans="2:68" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:109" ht="18.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="19"/>
       <c r="C39" s="19"/>
       <c r="D39" s="19"/>
@@ -3588,8 +4200,49 @@
       <c r="BN39" s="19"/>
       <c r="BO39" s="19"/>
       <c r="BP39" s="19"/>
+      <c r="BQ39" s="19"/>
+      <c r="BR39" s="19"/>
+      <c r="BS39" s="19"/>
+      <c r="BT39" s="19"/>
+      <c r="BU39" s="19"/>
+      <c r="BV39" s="19"/>
+      <c r="BW39" s="19"/>
+      <c r="BX39" s="19"/>
+      <c r="BY39" s="19"/>
+      <c r="BZ39" s="19"/>
+      <c r="CA39" s="19"/>
+      <c r="CB39" s="19"/>
+      <c r="CC39" s="19"/>
+      <c r="CD39" s="19"/>
+      <c r="CE39" s="19"/>
+      <c r="CF39" s="19"/>
+      <c r="CG39" s="19"/>
+      <c r="CH39" s="19"/>
+      <c r="CI39" s="19"/>
+      <c r="CJ39" s="19"/>
+      <c r="CK39" s="19"/>
+      <c r="CL39" s="19"/>
+      <c r="CM39" s="19"/>
+      <c r="CN39" s="19"/>
+      <c r="CO39" s="19"/>
+      <c r="CP39" s="19"/>
+      <c r="CQ39" s="19"/>
+      <c r="CR39" s="19"/>
+      <c r="CS39" s="19"/>
+      <c r="CT39" s="19"/>
+      <c r="CU39" s="19"/>
+      <c r="CV39" s="19"/>
+      <c r="CW39" s="19"/>
+      <c r="CX39" s="19"/>
+      <c r="CY39" s="19"/>
+      <c r="CZ39" s="19"/>
+      <c r="DA39" s="19"/>
+      <c r="DB39" s="19"/>
+      <c r="DC39" s="19"/>
+      <c r="DD39" s="19"/>
+      <c r="DE39" s="19"/>
     </row>
-    <row r="40" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:109" x14ac:dyDescent="0.3">
       <c r="B40" s="23"/>
       <c r="C40" s="24"/>
       <c r="D40" s="24"/>
@@ -3608,7 +4261,7 @@
       <c r="Q40" s="24"/>
       <c r="R40" s="24"/>
     </row>
-    <row r="41" spans="2:68" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:109" x14ac:dyDescent="0.3">
       <c r="B41" s="23"/>
       <c r="C41" s="24"/>
       <c r="D41" s="24"/>
@@ -3631,49 +4284,49 @@
   <mergeCells count="1">
     <mergeCell ref="B2:G4"/>
   </mergeCells>
-  <conditionalFormatting sqref="I13:BP39">
-    <cfRule type="expression" dxfId="26" priority="3">
+  <conditionalFormatting sqref="I13:DE39">
+    <cfRule type="expression" dxfId="7" priority="3">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="5">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="7">
+    <cfRule type="expression" dxfId="4" priority="7">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="8">
+    <cfRule type="expression" dxfId="3" priority="8">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="9">
+    <cfRule type="expression" dxfId="2" priority="9">
       <formula>I$12=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="13">
+    <cfRule type="expression" dxfId="1" priority="13">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="14">
+    <cfRule type="expression" dxfId="0" priority="14">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B40:BP40">
-    <cfRule type="expression" dxfId="18" priority="4">
+    <cfRule type="expression" dxfId="11" priority="4">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I12:BP12">
-    <cfRule type="expression" dxfId="17" priority="10">
+  <conditionalFormatting sqref="I12:DE12">
+    <cfRule type="expression" dxfId="8" priority="10">
       <formula>I$12=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O6">
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:BZ9">
-    <cfRule type="timePeriod" dxfId="1" priority="1" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="9" priority="1" timePeriod="today">
       <formula>FLOOR(I9,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>